<commit_message>
1.1 no submit buttons
</commit_message>
<xml_diff>
--- a/ResultGridConstruction.xlsx
+++ b/ResultGridConstruction.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samzimmerman/Documents/Apps/Macular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BDC1A3F-7D51-8A49-AA2C-A6C9335617D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008D59B3-E903-2042-9F02-C536DE4F7879}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{3063D372-EBC2-EA45-8402-FA27C249D01C}"/>
   </bookViews>
@@ -32,15 +32,38 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -82,13 +105,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -105,15 +128,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,14 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9844E8-ACC4-E341-A65E-37AE189FDC5D}">
-  <dimension ref="B3:T21"/>
+  <dimension ref="B3:T137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="20" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -971,61 +997,61 @@
       </c>
     </row>
     <row r="12" spans="2:20">
-      <c r="B12" s="6">
+      <c r="B12" s="8">
         <v>171</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="8">
         <v>172</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="8">
         <v>173</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="8">
         <v>174</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="8">
         <v>175</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="8">
         <v>176</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="8">
         <v>177</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="8">
         <v>178</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="8">
         <v>179</v>
       </c>
       <c r="K12" s="2">
         <v>180</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="9">
         <v>181</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="9">
         <v>182</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="9">
         <v>183</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="9">
         <v>184</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="9">
         <v>185</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="Q12" s="9">
         <v>186</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R12" s="9">
         <v>187</v>
       </c>
-      <c r="S12" s="7">
+      <c r="S12" s="9">
         <v>188</v>
       </c>
-      <c r="T12" s="7">
+      <c r="T12" s="9">
         <v>189</v>
       </c>
     </row>
@@ -1558,6 +1584,1621 @@
       </c>
       <c r="T21" s="5">
         <v>360</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20">
+      <c r="B26" s="6">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1</v>
+      </c>
+      <c r="D26" s="6">
+        <v>2</v>
+      </c>
+      <c r="E26" s="6">
+        <v>3</v>
+      </c>
+      <c r="F26" s="6">
+        <v>4</v>
+      </c>
+      <c r="G26" s="6">
+        <v>5</v>
+      </c>
+      <c r="H26" s="6">
+        <v>6</v>
+      </c>
+      <c r="I26" s="6">
+        <v>7</v>
+      </c>
+      <c r="J26" s="6">
+        <v>8</v>
+      </c>
+      <c r="K26" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20">
+      <c r="B27" s="1">
+        <v>10</v>
+      </c>
+      <c r="C27" s="1">
+        <v>11</v>
+      </c>
+      <c r="D27" s="1">
+        <v>12</v>
+      </c>
+      <c r="E27" s="1">
+        <v>13</v>
+      </c>
+      <c r="F27" s="1">
+        <v>14</v>
+      </c>
+      <c r="G27" s="1">
+        <v>15</v>
+      </c>
+      <c r="H27" s="1">
+        <v>16</v>
+      </c>
+      <c r="I27" s="1">
+        <v>17</v>
+      </c>
+      <c r="J27" s="1">
+        <v>18</v>
+      </c>
+      <c r="K27" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20">
+      <c r="B28" s="1">
+        <v>20</v>
+      </c>
+      <c r="C28" s="1">
+        <v>21</v>
+      </c>
+      <c r="D28" s="1">
+        <v>22</v>
+      </c>
+      <c r="E28" s="1">
+        <v>23</v>
+      </c>
+      <c r="F28" s="1">
+        <v>24</v>
+      </c>
+      <c r="G28" s="1">
+        <v>25</v>
+      </c>
+      <c r="H28" s="1">
+        <v>26</v>
+      </c>
+      <c r="I28" s="1">
+        <v>27</v>
+      </c>
+      <c r="J28" s="1">
+        <v>28</v>
+      </c>
+      <c r="K28" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20">
+      <c r="B29" s="1">
+        <v>30</v>
+      </c>
+      <c r="C29" s="1">
+        <v>31</v>
+      </c>
+      <c r="D29" s="1">
+        <v>32</v>
+      </c>
+      <c r="E29" s="1">
+        <v>33</v>
+      </c>
+      <c r="F29" s="1">
+        <v>34</v>
+      </c>
+      <c r="G29" s="1">
+        <v>35</v>
+      </c>
+      <c r="H29" s="1">
+        <v>36</v>
+      </c>
+      <c r="I29" s="1">
+        <v>37</v>
+      </c>
+      <c r="J29" s="1">
+        <v>38</v>
+      </c>
+      <c r="K29" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20">
+      <c r="B30" s="1">
+        <v>40</v>
+      </c>
+      <c r="C30" s="1">
+        <v>41</v>
+      </c>
+      <c r="D30" s="1">
+        <v>42</v>
+      </c>
+      <c r="E30" s="1">
+        <v>43</v>
+      </c>
+      <c r="F30" s="1">
+        <v>44</v>
+      </c>
+      <c r="G30" s="1">
+        <v>45</v>
+      </c>
+      <c r="H30" s="1">
+        <v>46</v>
+      </c>
+      <c r="I30" s="1">
+        <v>47</v>
+      </c>
+      <c r="J30" s="1">
+        <v>48</v>
+      </c>
+      <c r="K30" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20">
+      <c r="B31" s="1">
+        <v>50</v>
+      </c>
+      <c r="C31" s="1">
+        <v>51</v>
+      </c>
+      <c r="D31" s="1">
+        <v>52</v>
+      </c>
+      <c r="E31" s="1">
+        <v>53</v>
+      </c>
+      <c r="F31" s="1">
+        <v>54</v>
+      </c>
+      <c r="G31" s="1">
+        <v>55</v>
+      </c>
+      <c r="H31" s="1">
+        <v>56</v>
+      </c>
+      <c r="I31" s="1">
+        <v>57</v>
+      </c>
+      <c r="J31" s="1">
+        <v>58</v>
+      </c>
+      <c r="K31" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20">
+      <c r="B32" s="1">
+        <v>60</v>
+      </c>
+      <c r="C32" s="1">
+        <v>61</v>
+      </c>
+      <c r="D32" s="1">
+        <v>62</v>
+      </c>
+      <c r="E32" s="1">
+        <v>63</v>
+      </c>
+      <c r="F32" s="1">
+        <v>64</v>
+      </c>
+      <c r="G32" s="1">
+        <v>65</v>
+      </c>
+      <c r="H32" s="1">
+        <v>66</v>
+      </c>
+      <c r="I32" s="1">
+        <v>67</v>
+      </c>
+      <c r="J32" s="1">
+        <v>68</v>
+      </c>
+      <c r="K32" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11">
+      <c r="B33" s="1">
+        <v>70</v>
+      </c>
+      <c r="C33" s="1">
+        <v>71</v>
+      </c>
+      <c r="D33" s="1">
+        <v>72</v>
+      </c>
+      <c r="E33" s="1">
+        <v>73</v>
+      </c>
+      <c r="F33" s="1">
+        <v>74</v>
+      </c>
+      <c r="G33" s="1">
+        <v>75</v>
+      </c>
+      <c r="H33" s="1">
+        <v>76</v>
+      </c>
+      <c r="I33" s="1">
+        <v>77</v>
+      </c>
+      <c r="J33" s="1">
+        <v>78</v>
+      </c>
+      <c r="K33" s="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11">
+      <c r="B34" s="1">
+        <v>80</v>
+      </c>
+      <c r="C34" s="1">
+        <v>81</v>
+      </c>
+      <c r="D34" s="1">
+        <v>82</v>
+      </c>
+      <c r="E34" s="1">
+        <v>83</v>
+      </c>
+      <c r="F34" s="1">
+        <v>84</v>
+      </c>
+      <c r="G34" s="1">
+        <v>85</v>
+      </c>
+      <c r="H34" s="1">
+        <v>86</v>
+      </c>
+      <c r="I34" s="1">
+        <v>87</v>
+      </c>
+      <c r="J34" s="1">
+        <v>88</v>
+      </c>
+      <c r="K34" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11">
+      <c r="B35" s="1">
+        <v>90</v>
+      </c>
+      <c r="C35" s="1">
+        <v>91</v>
+      </c>
+      <c r="D35" s="1">
+        <v>92</v>
+      </c>
+      <c r="E35" s="1">
+        <v>93</v>
+      </c>
+      <c r="F35" s="1">
+        <v>94</v>
+      </c>
+      <c r="G35" s="1">
+        <v>95</v>
+      </c>
+      <c r="H35" s="1">
+        <v>96</v>
+      </c>
+      <c r="I35" s="1">
+        <v>97</v>
+      </c>
+      <c r="J35" s="1">
+        <v>98</v>
+      </c>
+      <c r="K35" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11">
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11">
+      <c r="C38" s="7"/>
+      <c r="D38">
+        <v>19</v>
+      </c>
+      <c r="E38" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11">
+      <c r="C39" s="7">
+        <v>89</v>
+      </c>
+      <c r="D39">
+        <v>18</v>
+      </c>
+      <c r="E39" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11">
+      <c r="B40">
+        <v>91</v>
+      </c>
+      <c r="C40" s="7">
+        <v>98</v>
+      </c>
+      <c r="D40">
+        <v>29</v>
+      </c>
+      <c r="E40" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11">
+      <c r="C41" s="7">
+        <v>79</v>
+      </c>
+      <c r="D41">
+        <v>17</v>
+      </c>
+      <c r="E41" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11">
+      <c r="B42">
+        <v>81</v>
+      </c>
+      <c r="C42" s="7">
+        <v>88</v>
+      </c>
+      <c r="D42">
+        <v>28</v>
+      </c>
+      <c r="E42" s="7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11">
+      <c r="B43">
+        <v>92</v>
+      </c>
+      <c r="C43" s="7">
+        <v>97</v>
+      </c>
+      <c r="D43">
+        <v>39</v>
+      </c>
+      <c r="E43" s="7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11">
+      <c r="C44" s="7">
+        <v>69</v>
+      </c>
+      <c r="D44">
+        <v>16</v>
+      </c>
+      <c r="E44" s="7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11">
+      <c r="B45">
+        <v>71</v>
+      </c>
+      <c r="C45" s="7">
+        <v>78</v>
+      </c>
+      <c r="D45">
+        <v>27</v>
+      </c>
+      <c r="E45" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11">
+      <c r="B46">
+        <v>82</v>
+      </c>
+      <c r="C46" s="7">
+        <v>87</v>
+      </c>
+      <c r="D46">
+        <v>38</v>
+      </c>
+      <c r="E46" s="7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11">
+      <c r="B47">
+        <v>93</v>
+      </c>
+      <c r="C47" s="7">
+        <v>96</v>
+      </c>
+      <c r="D47">
+        <v>49</v>
+      </c>
+      <c r="E47" s="7">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11">
+      <c r="C48" s="7">
+        <v>59</v>
+      </c>
+      <c r="D48">
+        <v>15</v>
+      </c>
+      <c r="E48" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="B49">
+        <v>61</v>
+      </c>
+      <c r="C49" s="7">
+        <v>68</v>
+      </c>
+      <c r="D49">
+        <v>26</v>
+      </c>
+      <c r="E49" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5">
+      <c r="B50">
+        <v>72</v>
+      </c>
+      <c r="C50" s="7">
+        <v>77</v>
+      </c>
+      <c r="D50">
+        <v>37</v>
+      </c>
+      <c r="E50" s="7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5">
+      <c r="B51">
+        <v>83</v>
+      </c>
+      <c r="C51" s="7">
+        <v>86</v>
+      </c>
+      <c r="D51">
+        <v>48</v>
+      </c>
+      <c r="E51" s="7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5">
+      <c r="B52">
+        <v>94</v>
+      </c>
+      <c r="C52" s="7">
+        <v>95</v>
+      </c>
+      <c r="D52">
+        <v>59</v>
+      </c>
+      <c r="E52" s="7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5">
+      <c r="C53" s="7">
+        <v>49</v>
+      </c>
+      <c r="D53">
+        <v>14</v>
+      </c>
+      <c r="E53" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5">
+      <c r="B54">
+        <v>51</v>
+      </c>
+      <c r="C54" s="7">
+        <v>58</v>
+      </c>
+      <c r="D54">
+        <v>25</v>
+      </c>
+      <c r="E54" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5">
+      <c r="B55">
+        <v>62</v>
+      </c>
+      <c r="C55" s="7">
+        <v>67</v>
+      </c>
+      <c r="D55">
+        <v>36</v>
+      </c>
+      <c r="E55" s="7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5">
+      <c r="B56">
+        <v>73</v>
+      </c>
+      <c r="C56" s="7">
+        <v>76</v>
+      </c>
+      <c r="D56">
+        <v>47</v>
+      </c>
+      <c r="E56" s="7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5">
+      <c r="B57">
+        <v>84</v>
+      </c>
+      <c r="C57" s="7">
+        <v>85</v>
+      </c>
+      <c r="D57">
+        <v>58</v>
+      </c>
+      <c r="E57" s="7">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5">
+      <c r="B58">
+        <v>95</v>
+      </c>
+      <c r="C58" s="7">
+        <v>94</v>
+      </c>
+      <c r="D58">
+        <v>69</v>
+      </c>
+      <c r="E58" s="7">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5">
+      <c r="C59" s="7">
+        <v>39</v>
+      </c>
+      <c r="D59">
+        <v>13</v>
+      </c>
+      <c r="E59" s="7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5">
+      <c r="B60">
+        <v>41</v>
+      </c>
+      <c r="C60" s="7">
+        <v>48</v>
+      </c>
+      <c r="D60">
+        <v>24</v>
+      </c>
+      <c r="E60" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5">
+      <c r="B61">
+        <v>52</v>
+      </c>
+      <c r="C61" s="7">
+        <v>57</v>
+      </c>
+      <c r="D61">
+        <v>35</v>
+      </c>
+      <c r="E61" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5">
+      <c r="B62">
+        <v>63</v>
+      </c>
+      <c r="C62" s="7">
+        <v>66</v>
+      </c>
+      <c r="D62">
+        <v>46</v>
+      </c>
+      <c r="E62" s="7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5">
+      <c r="B63">
+        <v>74</v>
+      </c>
+      <c r="C63" s="7">
+        <v>75</v>
+      </c>
+      <c r="D63">
+        <v>57</v>
+      </c>
+      <c r="E63" s="7">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5">
+      <c r="B64">
+        <v>85</v>
+      </c>
+      <c r="C64" s="7">
+        <v>84</v>
+      </c>
+      <c r="D64">
+        <v>68</v>
+      </c>
+      <c r="E64" s="7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5">
+      <c r="B65">
+        <v>96</v>
+      </c>
+      <c r="C65" s="7">
+        <v>93</v>
+      </c>
+      <c r="D65">
+        <v>79</v>
+      </c>
+      <c r="E65" s="7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5">
+      <c r="C66" s="7">
+        <v>29</v>
+      </c>
+      <c r="D66">
+        <v>12</v>
+      </c>
+      <c r="E66" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5">
+      <c r="B67">
+        <v>31</v>
+      </c>
+      <c r="C67" s="7">
+        <v>38</v>
+      </c>
+      <c r="D67">
+        <v>23</v>
+      </c>
+      <c r="E67" s="7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5">
+      <c r="B68">
+        <v>42</v>
+      </c>
+      <c r="C68" s="7">
+        <v>47</v>
+      </c>
+      <c r="D68">
+        <v>34</v>
+      </c>
+      <c r="E68" s="7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5">
+      <c r="B69">
+        <v>53</v>
+      </c>
+      <c r="C69" s="7">
+        <v>56</v>
+      </c>
+      <c r="D69">
+        <v>45</v>
+      </c>
+      <c r="E69" s="7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5">
+      <c r="B70">
+        <v>64</v>
+      </c>
+      <c r="C70" s="7">
+        <v>65</v>
+      </c>
+      <c r="D70">
+        <v>56</v>
+      </c>
+      <c r="E70" s="7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5">
+      <c r="B71">
+        <v>75</v>
+      </c>
+      <c r="C71" s="7">
+        <v>74</v>
+      </c>
+      <c r="D71">
+        <v>67</v>
+      </c>
+      <c r="E71" s="7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5">
+      <c r="B72">
+        <v>86</v>
+      </c>
+      <c r="C72" s="7">
+        <v>83</v>
+      </c>
+      <c r="D72">
+        <v>78</v>
+      </c>
+      <c r="E72" s="7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5">
+      <c r="B73">
+        <v>97</v>
+      </c>
+      <c r="C73" s="7">
+        <v>92</v>
+      </c>
+      <c r="D73">
+        <v>89</v>
+      </c>
+      <c r="E73" s="7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5">
+      <c r="C74" s="7">
+        <v>19</v>
+      </c>
+      <c r="D74">
+        <v>11</v>
+      </c>
+      <c r="E74" s="7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5">
+      <c r="B75">
+        <v>21</v>
+      </c>
+      <c r="C75" s="7">
+        <v>28</v>
+      </c>
+      <c r="D75">
+        <v>22</v>
+      </c>
+      <c r="E75" s="7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5">
+      <c r="B76">
+        <v>32</v>
+      </c>
+      <c r="C76" s="7">
+        <v>37</v>
+      </c>
+      <c r="D76">
+        <v>33</v>
+      </c>
+      <c r="E76" s="7">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5">
+      <c r="B77">
+        <v>43</v>
+      </c>
+      <c r="C77" s="7">
+        <v>46</v>
+      </c>
+      <c r="D77">
+        <v>44</v>
+      </c>
+      <c r="E77" s="7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5">
+      <c r="B78">
+        <v>54</v>
+      </c>
+      <c r="C78" s="7">
+        <v>55</v>
+      </c>
+      <c r="D78">
+        <v>55</v>
+      </c>
+      <c r="E78" s="7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5">
+      <c r="B79">
+        <v>65</v>
+      </c>
+      <c r="C79" s="7">
+        <v>64</v>
+      </c>
+      <c r="D79">
+        <v>66</v>
+      </c>
+      <c r="E79" s="7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5">
+      <c r="B80">
+        <v>76</v>
+      </c>
+      <c r="C80" s="7">
+        <v>73</v>
+      </c>
+      <c r="D80">
+        <v>77</v>
+      </c>
+      <c r="E80" s="7">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5">
+      <c r="B81">
+        <v>87</v>
+      </c>
+      <c r="C81" s="7">
+        <v>82</v>
+      </c>
+      <c r="D81">
+        <v>88</v>
+      </c>
+      <c r="E81" s="7">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5">
+      <c r="B82">
+        <v>98</v>
+      </c>
+      <c r="C82" s="7">
+        <v>91</v>
+      </c>
+      <c r="D82">
+        <v>99</v>
+      </c>
+      <c r="E82" s="7">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5">
+      <c r="C83" s="7">
+        <v>9</v>
+      </c>
+      <c r="D83">
+        <v>10</v>
+      </c>
+      <c r="E83" s="7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5">
+      <c r="B84">
+        <v>11</v>
+      </c>
+      <c r="C84" s="7">
+        <v>18</v>
+      </c>
+      <c r="D84">
+        <v>21</v>
+      </c>
+      <c r="E84" s="7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5">
+      <c r="B85">
+        <v>22</v>
+      </c>
+      <c r="C85" s="7">
+        <v>27</v>
+      </c>
+      <c r="D85">
+        <v>32</v>
+      </c>
+      <c r="E85" s="7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5">
+      <c r="B86">
+        <v>33</v>
+      </c>
+      <c r="C86" s="7">
+        <v>36</v>
+      </c>
+      <c r="D86">
+        <v>43</v>
+      </c>
+      <c r="E86" s="7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5">
+      <c r="B87">
+        <v>44</v>
+      </c>
+      <c r="C87" s="7">
+        <v>45</v>
+      </c>
+      <c r="D87">
+        <v>54</v>
+      </c>
+      <c r="E87" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5">
+      <c r="B88">
+        <v>55</v>
+      </c>
+      <c r="C88" s="7">
+        <v>54</v>
+      </c>
+      <c r="D88">
+        <v>65</v>
+      </c>
+      <c r="E88" s="7">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5">
+      <c r="B89">
+        <v>66</v>
+      </c>
+      <c r="C89" s="7">
+        <v>63</v>
+      </c>
+      <c r="D89">
+        <v>76</v>
+      </c>
+      <c r="E89" s="7">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5">
+      <c r="B90">
+        <v>77</v>
+      </c>
+      <c r="C90" s="7">
+        <v>72</v>
+      </c>
+      <c r="D90">
+        <v>87</v>
+      </c>
+      <c r="E90" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5">
+      <c r="B91">
+        <v>88</v>
+      </c>
+      <c r="C91" s="7">
+        <v>81</v>
+      </c>
+      <c r="D91">
+        <v>98</v>
+      </c>
+      <c r="E91" s="7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5">
+      <c r="B92">
+        <v>99</v>
+      </c>
+      <c r="C92" s="7">
+        <v>90</v>
+      </c>
+      <c r="D92" s="7">
+        <v>20</v>
+      </c>
+      <c r="E92" s="7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5">
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93" s="7">
+        <v>8</v>
+      </c>
+      <c r="D93" s="7">
+        <v>31</v>
+      </c>
+      <c r="E93" s="7">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5">
+      <c r="B94">
+        <v>12</v>
+      </c>
+      <c r="C94" s="7">
+        <v>17</v>
+      </c>
+      <c r="D94" s="7">
+        <v>42</v>
+      </c>
+      <c r="E94" s="7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5">
+      <c r="B95">
+        <v>23</v>
+      </c>
+      <c r="C95" s="7">
+        <v>26</v>
+      </c>
+      <c r="D95" s="7">
+        <v>53</v>
+      </c>
+      <c r="E95" s="7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5">
+      <c r="B96">
+        <v>34</v>
+      </c>
+      <c r="C96" s="7">
+        <v>35</v>
+      </c>
+      <c r="D96" s="7">
+        <v>64</v>
+      </c>
+      <c r="E96" s="7">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5">
+      <c r="B97">
+        <v>45</v>
+      </c>
+      <c r="C97" s="7">
+        <v>44</v>
+      </c>
+      <c r="D97" s="7">
+        <v>75</v>
+      </c>
+      <c r="E97" s="7">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5">
+      <c r="B98">
+        <v>56</v>
+      </c>
+      <c r="C98" s="7">
+        <v>53</v>
+      </c>
+      <c r="D98" s="7">
+        <v>86</v>
+      </c>
+      <c r="E98" s="7">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5">
+      <c r="B99">
+        <v>67</v>
+      </c>
+      <c r="C99" s="7">
+        <v>62</v>
+      </c>
+      <c r="D99" s="7">
+        <v>97</v>
+      </c>
+      <c r="E99" s="7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5">
+      <c r="B100">
+        <v>78</v>
+      </c>
+      <c r="C100" s="7">
+        <v>71</v>
+      </c>
+      <c r="D100" s="7">
+        <v>30</v>
+      </c>
+      <c r="E100" s="7">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5">
+      <c r="B101">
+        <v>89</v>
+      </c>
+      <c r="C101" s="7">
+        <v>80</v>
+      </c>
+      <c r="D101" s="7">
+        <v>41</v>
+      </c>
+      <c r="E101" s="7">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5">
+      <c r="B102">
+        <v>2</v>
+      </c>
+      <c r="C102" s="7">
+        <v>7</v>
+      </c>
+      <c r="D102" s="7">
+        <v>52</v>
+      </c>
+      <c r="E102" s="7">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5">
+      <c r="B103">
+        <v>13</v>
+      </c>
+      <c r="C103" s="7">
+        <v>16</v>
+      </c>
+      <c r="D103" s="7">
+        <v>63</v>
+      </c>
+      <c r="E103" s="7">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5">
+      <c r="B104">
+        <v>24</v>
+      </c>
+      <c r="C104" s="7">
+        <v>25</v>
+      </c>
+      <c r="D104" s="7">
+        <v>74</v>
+      </c>
+      <c r="E104" s="7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5">
+      <c r="B105">
+        <v>35</v>
+      </c>
+      <c r="C105" s="7">
+        <v>34</v>
+      </c>
+      <c r="D105" s="7">
+        <v>85</v>
+      </c>
+      <c r="E105" s="7">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5">
+      <c r="B106">
+        <v>46</v>
+      </c>
+      <c r="C106" s="7">
+        <v>43</v>
+      </c>
+      <c r="D106" s="7">
+        <v>96</v>
+      </c>
+      <c r="E106" s="7">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5">
+      <c r="B107">
+        <v>57</v>
+      </c>
+      <c r="C107" s="7">
+        <v>52</v>
+      </c>
+      <c r="D107" s="7">
+        <v>40</v>
+      </c>
+      <c r="E107" s="7">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5">
+      <c r="B108">
+        <v>68</v>
+      </c>
+      <c r="C108" s="7">
+        <v>61</v>
+      </c>
+      <c r="D108" s="7">
+        <v>51</v>
+      </c>
+      <c r="E108" s="7">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5">
+      <c r="B109">
+        <v>79</v>
+      </c>
+      <c r="C109" s="7">
+        <v>70</v>
+      </c>
+      <c r="D109" s="7">
+        <v>62</v>
+      </c>
+      <c r="E109" s="7">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5">
+      <c r="B110">
+        <v>3</v>
+      </c>
+      <c r="C110" s="7">
+        <v>6</v>
+      </c>
+      <c r="D110" s="7">
+        <v>73</v>
+      </c>
+      <c r="E110" s="7">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5">
+      <c r="B111">
+        <v>14</v>
+      </c>
+      <c r="C111" s="7">
+        <v>15</v>
+      </c>
+      <c r="D111" s="7">
+        <v>84</v>
+      </c>
+      <c r="E111" s="7">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5">
+      <c r="B112">
+        <v>25</v>
+      </c>
+      <c r="C112" s="7">
+        <v>24</v>
+      </c>
+      <c r="D112" s="7">
+        <v>95</v>
+      </c>
+      <c r="E112" s="7">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5">
+      <c r="B113">
+        <v>36</v>
+      </c>
+      <c r="C113" s="7">
+        <v>33</v>
+      </c>
+      <c r="D113" s="7">
+        <v>50</v>
+      </c>
+      <c r="E113" s="7">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5">
+      <c r="B114">
+        <v>47</v>
+      </c>
+      <c r="C114" s="7">
+        <v>42</v>
+      </c>
+      <c r="D114" s="7">
+        <v>61</v>
+      </c>
+      <c r="E114" s="7">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5">
+      <c r="B115">
+        <v>58</v>
+      </c>
+      <c r="C115" s="7">
+        <v>51</v>
+      </c>
+      <c r="D115" s="7">
+        <v>72</v>
+      </c>
+      <c r="E115" s="7">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5">
+      <c r="B116">
+        <v>69</v>
+      </c>
+      <c r="C116" s="7">
+        <v>60</v>
+      </c>
+      <c r="D116" s="7">
+        <v>83</v>
+      </c>
+      <c r="E116" s="7">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5">
+      <c r="B117">
+        <v>4</v>
+      </c>
+      <c r="C117" s="7">
+        <v>5</v>
+      </c>
+      <c r="D117" s="7">
+        <v>94</v>
+      </c>
+      <c r="E117" s="7">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5">
+      <c r="B118">
+        <v>15</v>
+      </c>
+      <c r="C118" s="7">
+        <v>14</v>
+      </c>
+      <c r="D118" s="7">
+        <v>60</v>
+      </c>
+      <c r="E118" s="7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5">
+      <c r="B119">
+        <v>26</v>
+      </c>
+      <c r="C119" s="7">
+        <v>23</v>
+      </c>
+      <c r="D119" s="7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5">
+      <c r="B120">
+        <v>37</v>
+      </c>
+      <c r="C120" s="7">
+        <v>32</v>
+      </c>
+      <c r="D120" s="7">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5">
+      <c r="B121">
+        <v>48</v>
+      </c>
+      <c r="C121" s="7">
+        <v>41</v>
+      </c>
+      <c r="D121" s="7">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5">
+      <c r="B122">
+        <v>59</v>
+      </c>
+      <c r="C122" s="7">
+        <v>50</v>
+      </c>
+      <c r="D122" s="7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5">
+      <c r="B123">
+        <v>5</v>
+      </c>
+      <c r="C123" s="7">
+        <v>4</v>
+      </c>
+      <c r="D123" s="7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5">
+      <c r="B124">
+        <v>16</v>
+      </c>
+      <c r="C124" s="7">
+        <v>13</v>
+      </c>
+      <c r="D124" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5">
+      <c r="B125">
+        <v>27</v>
+      </c>
+      <c r="C125" s="7">
+        <v>22</v>
+      </c>
+      <c r="D125" s="7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5">
+      <c r="B126">
+        <v>38</v>
+      </c>
+      <c r="C126" s="7">
+        <v>31</v>
+      </c>
+      <c r="D126" s="7">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5">
+      <c r="B127">
+        <v>49</v>
+      </c>
+      <c r="C127" s="7">
+        <v>40</v>
+      </c>
+      <c r="D127" s="7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5">
+      <c r="B128">
+        <v>6</v>
+      </c>
+      <c r="C128" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3">
+      <c r="B129">
+        <v>17</v>
+      </c>
+      <c r="C129" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3">
+      <c r="B130">
+        <v>28</v>
+      </c>
+      <c r="C130" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3">
+      <c r="B131">
+        <v>39</v>
+      </c>
+      <c r="C131" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3">
+      <c r="B132">
+        <v>7</v>
+      </c>
+      <c r="C132" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3">
+      <c r="B133">
+        <v>18</v>
+      </c>
+      <c r="C133" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3">
+      <c r="B134">
+        <v>29</v>
+      </c>
+      <c r="C134" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3">
+      <c r="B135">
+        <v>8</v>
+      </c>
+      <c r="C135" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3">
+      <c r="B136">
+        <v>19</v>
+      </c>
+      <c r="C136" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3">
+      <c r="B137">
+        <v>9</v>
+      </c>
+      <c r="C137" s="7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>